<commit_message>
merger to new branch
</commit_message>
<xml_diff>
--- a/1stpackage/Data.xlsx
+++ b/1stpackage/Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EI12548\PycharmProjects\AutomateWebpage\1stpackage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EI12548\PycharmProjects\pythonProject\Cloned project\python_selenium_demo\1stpackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB19FAE-DCF2-46DF-9483-ACD69CCDD33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D30FA-A373-45E9-A5E9-0F7ECC9FE926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ramya</t>
   </si>
   <si>
     <t>soumya</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -350,7 +354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -375,4 +379,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA046C1-D650-479B-A34F-77F842006309}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>